<commit_message>
Fix lỗi update data
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programing\C\atm-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2693BCD6-A465-471E-BB77-8F646BCDB2D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE62F711-41C4-4DC5-A87F-D742CFF31591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E96742D2-17DD-497A-8372-42FD2924433A}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{E96742D2-17DD-497A-8372-42FD2924433A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>001</t>
   </si>
@@ -129,13 +130,46 @@
   </si>
   <si>
     <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Tài khoản</t>
+  </si>
+  <si>
+    <t>Mật Khẩu</t>
+  </si>
+  <si>
+    <t>Họ Tên</t>
+  </si>
+  <si>
+    <t>nv1</t>
+  </si>
+  <si>
+    <t>Nhân viên 1</t>
+  </si>
+  <si>
+    <t>nv2</t>
+  </si>
+  <si>
+    <t>nv3</t>
+  </si>
+  <si>
+    <t>nv4</t>
+  </si>
+  <si>
+    <t>Nhân viên 2</t>
+  </si>
+  <si>
+    <t>Nhân viên 3</t>
+  </si>
+  <si>
+    <t>Nhân viên 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +186,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -178,13 +220,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F748D47-E4C8-4067-9E9C-6DA2238409BF}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,4 +799,96 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377E0E52-C3DD-4C5E-B4BA-422C389E2F0D}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>